<commit_message>
final project part 1 submitted
</commit_message>
<xml_diff>
--- a/final/worky.xlsx
+++ b/final/worky.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\source\repos\ds700\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E73D50B1-BBBA-4639-B821-4FB09FE59B8B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{2309470D-F95D-4BC4-A54A-AE231E1D00F7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6912" activeTab="1" xr2:uid="{BD6714F2-7C40-45CA-9A5A-A5F572D551EB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6912" xr2:uid="{BD6714F2-7C40-45CA-9A5A-A5F572D551EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A5589E-3CFD-477A-B53F-E7DEE0AF98EA}">
   <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8:W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,10 +592,10 @@
         <v>6084.6719999999996</v>
       </c>
       <c r="P8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="U8" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="U8" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
@@ -1143,7 +1143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C7A5BB-D210-4C16-B50F-2B22985E034A}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:I7"/>
     </sheetView>
   </sheetViews>

</xml_diff>